<commit_message>
revert v1.1.5 wrong release
</commit_message>
<xml_diff>
--- a/trust/CodeSystem-WHO.TRUST.ACTOR.xlsx
+++ b/trust/CodeSystem-WHO.TRUST.ACTOR.xlsx
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>1.1.6</t>
+    <t>1.1.4</t>
   </si>
   <si>
     <t>Name</t>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-12-19T12:46:28+00:00</t>
+    <t>2024-11-04T12:37:06+00:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>